<commit_message>
nothing just a test
</commit_message>
<xml_diff>
--- a/Kangaroo/Resualt/Resualt.xlsx
+++ b/Kangaroo/Resualt/Resualt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harek\Documents\TalashExams\Kangaroo\Resualt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3933DC58-5607-49DF-89E7-6A870E6336D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897DB90D-13AD-407C-B827-29DAB837A7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FD5A05D5-3ECA-4382-B9BB-08A55F8B9F08}"/>
   </bookViews>
@@ -911,7 +911,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>